<commit_message>
fixed bug of empty rows
</commit_message>
<xml_diff>
--- a/sp500-historical-components-and-changes/sp500_regular_add.xlsx
+++ b/sp500-historical-components-and-changes/sp500_regular_add.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yingchen\Documents\GitHub\analyzingalpha\sp500-historical-components-and-changes\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16DA16B2-A100-4D9B-B43B-467D922B6275}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="18276" windowHeight="10992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Population Statistics" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>original_date</t>
   </si>
@@ -23,16 +29,19 @@
     <t>total</t>
   </si>
   <si>
+    <t>up</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
     <t>mean</t>
   </si>
   <si>
     <t>std</t>
-  </si>
-  <si>
-    <t>up</t>
-  </si>
-  <si>
-    <t>count</t>
   </si>
   <si>
     <t>max</t>
@@ -50,11 +59,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,9 +115,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -118,6 +130,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -164,7 +184,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -196,9 +216,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -230,6 +268,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -405,14 +461,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="2" width="17.41796875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -425,209 +487,183 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="1">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="2">
+        <v>42809</v>
+      </c>
+      <c r="D2">
         <v>0</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="2">
+        <v>42811</v>
+      </c>
+      <c r="B3" s="3">
         <v>42814</v>
       </c>
       <c r="C3">
         <v>0.2299919128417969</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="1">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="2">
+        <v>42887</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="2">
+        <v>42902</v>
+      </c>
+      <c r="B5" s="3">
+        <v>42905</v>
+      </c>
+      <c r="C5">
+        <v>4.9699935913085938</v>
+      </c>
+      <c r="D5">
         <v>3</v>
       </c>
-      <c r="B5" s="2">
-        <v>42905</v>
-      </c>
-      <c r="C5">
-        <v>4.969993591308594</v>
-      </c>
-      <c r="F5">
-        <v>3</v>
-      </c>
-      <c r="G5">
+      <c r="E5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="2">
+        <v>42978</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="2">
+        <v>42993</v>
+      </c>
+      <c r="B7" s="3">
         <v>42996</v>
       </c>
       <c r="C7">
         <v>0.25</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="2">
+        <v>43165</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="2">
+        <v>43175</v>
+      </c>
+      <c r="B9" s="3">
         <v>43178</v>
       </c>
       <c r="C9">
-        <v>3.409996032714844</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2">
+        <v>3.4099960327148442</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="2">
+        <v>43257</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="2">
+        <v>43266</v>
+      </c>
+      <c r="B11" s="3">
         <v>43269</v>
       </c>
       <c r="C11">
-        <v>-1.169998168945312</v>
-      </c>
-      <c r="F11">
+        <v>-1.1699981689453121</v>
+      </c>
+      <c r="D11">
         <v>0</v>
       </c>
-      <c r="G11">
+      <c r="E11">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12" s="2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="2">
+        <v>43455</v>
+      </c>
+      <c r="B12" s="3">
         <v>43458</v>
       </c>
       <c r="C12">
         <v>-1.819999694824219</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="F13">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="2">
+        <v>43685</v>
+      </c>
+      <c r="D13">
         <v>2</v>
       </c>
-      <c r="G13">
+      <c r="E13">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="2">
+        <v>43728</v>
+      </c>
+      <c r="B14" s="3">
         <v>43731</v>
       </c>
       <c r="C14">
         <v>-0.7400054931640625</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="1">
-        <v>13</v>
-      </c>
-      <c r="B15" s="2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="2">
+        <v>43819</v>
+      </c>
+      <c r="B15" s="3">
         <v>43822</v>
       </c>
       <c r="C15">
         <v>0.80999755859375</v>
       </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="1">
-        <v>14</v>
-      </c>
-      <c r="D16">
-        <v>0.3494103375603171</v>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -636,73 +672,73 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>5.939975738525391</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>5.9399757385253906</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.3494103375603171</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="B4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>0.34941033756031709</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10">
         <v>0.6470588235294118</v>

</xml_diff>